<commit_message>
modified analytical model and added an attempt to derive asymptotic formulas
</commit_message>
<xml_diff>
--- a/data/Modello Analitico.xlsx
+++ b/data/Modello Analitico.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniroma2-my.sharepoint.com/personal/livia_simoncini_alumni_uniroma2_eu/Documents/Corsi/Attivi/PMCSN/Progetto/PMCSN_Project/data/livia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniroma2-my.sharepoint.com/personal/livia_simoncini_alumni_uniroma2_eu/Documents/Corsi/Attivi/PMCSN/Progetto/PMCSN_Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="533" documentId="11_B2CD3B23B734BEB69962A3A2F81BCE609405F408" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6859DD76-4D42-4798-B59C-5345A6B817C1}"/>
+  <xr:revisionPtr revIDLastSave="550" documentId="11_B2CD3B23B734BEB69962A3A2F81BCE609405F408" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51E93B70-9450-4D7F-95D8-AC56B5F27DB5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dati_OPTN" sheetId="1" r:id="rId1"/>
     <sheet name="Arrivi" sheetId="2" r:id="rId2"/>
     <sheet name="Uscite" sheetId="3" r:id="rId3"/>
     <sheet name="Centri - Identical" sheetId="4" r:id="rId4"/>
-    <sheet name="Note" sheetId="7" r:id="rId5"/>
+    <sheet name="Foglio1" sheetId="8" r:id="rId5"/>
+    <sheet name="Note" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -100,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="84">
   <si>
     <t>PAZIENTI - ARRIVI</t>
   </si>
@@ -249,9 +250,6 @@
     <t>d/giorno (2014-2019)</t>
   </si>
   <si>
-    <t>P(Bt AND Pr)</t>
-  </si>
-  <si>
     <t>r/anno (2014-2019)</t>
   </si>
   <si>
@@ -333,10 +331,28 @@
     <t>Tasso d'ingresso totale</t>
   </si>
   <si>
-    <t>P(Bt | Pr)</t>
+    <t>Activation center</t>
   </si>
   <si>
-    <t>P(Pr | Bt)</t>
+    <t>Tasso di completamento</t>
+  </si>
+  <si>
+    <t>Waiting List</t>
+  </si>
+  <si>
+    <t>Organ Bank</t>
+  </si>
+  <si>
+    <t>Matching</t>
+  </si>
+  <si>
+    <t>Probabilità</t>
+  </si>
+  <si>
+    <t>Probabilità di morte</t>
+  </si>
+  <si>
+    <t>Probabilità di renege</t>
   </si>
 </sst>
 </file>
@@ -348,7 +364,7 @@
     <numFmt numFmtId="165" formatCode="0.00000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -392,8 +408,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -466,8 +488,68 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor rgb="FFDAE3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor rgb="FF99CCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor rgb="FFE2F0D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFC5E0B4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFF4B183"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFD0CECE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFDAE3F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -573,11 +655,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -633,7 +804,6 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -660,6 +830,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -695,10 +916,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -716,22 +937,38 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="22" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="165" formatCode="0.00000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -927,17 +1164,15 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabella5" displayName="Tabella5" ref="A2:G22" totalsRowShown="0">
-  <autoFilter ref="A2:G22" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Tabella5" displayName="Tabella5" ref="A2:E22" totalsRowShown="0">
+  <autoFilter ref="A2:E22" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="ABO"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Priorità"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="d/anno (2014-2019)"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="d/giorno (2014-2019)"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="P(Bt AND Pr)"/>
-    <tableColumn id="6" xr3:uid="{BA9696CB-973E-4C10-A048-3F2E161E3E03}" name="P(Bt | Pr)"/>
-    <tableColumn id="7" xr3:uid="{556A604F-B354-4937-B17D-BE37408A5600}" name="P(Pr | Bt)">
-      <calculatedColumnFormula>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</calculatedColumnFormula>
+    <tableColumn id="8" xr3:uid="{A87F9785-8BDD-4C18-9179-285F88A533E8}" name="Probabilità" dataDxfId="1">
+      <calculatedColumnFormula>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -945,34 +1180,19 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabella511" displayName="Tabella511" ref="A25:G45" totalsRowShown="0">
-  <autoFilter ref="A25:G45" xr:uid="{00000000-0009-0000-0100-000006000000}">
-    <filterColumn colId="0">
-      <filters blank="1">
-        <filter val="A"/>
-        <filter val="AB"/>
-        <filter val="B"/>
-        <filter val="O"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Tabella511" displayName="Tabella511" ref="A25:E45" totalsRowShown="0">
+  <autoFilter ref="A25:E45" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="ABO"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Priorità"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="r/anno (2014-2019)">
-      <calculatedColumnFormula>AVERAGE(Dati_OPTN!Q49:V49)</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(AVERAGE(Dati_OPTN!Q49:V49) &gt; Arrivi!C3, Arrivi!C3, AVERAGE(Dati_OPTN!Q49:V49))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="r/giorno (2014-2019)">
       <calculatedColumnFormula>Tabella511[[#This Row],[r/anno (2014-2019)]]/365</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="P(Bt AND Pr)">
-      <calculatedColumnFormula>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{E91D55C8-AA3E-42C5-9822-44CC27598042}" name="P(Bt | Pr)">
-      <calculatedColumnFormula>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{FA8A30BA-728B-45BF-9A31-1E3623916B71}" name="P(Pr | Bt)">
-      <calculatedColumnFormula>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Probabilità">
+      <calculatedColumnFormula>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -980,22 +1200,16 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Tabella512" displayName="Tabella512" ref="A49:G69" totalsRowShown="0">
-  <autoFilter ref="A49:G69" xr:uid="{00000000-0009-0000-0100-000007000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="All Types"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Tabella512" displayName="Tabella512" ref="A49:E69" totalsRowShown="0">
+  <autoFilter ref="A49:E69" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="ABO"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Priorità"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="t/anno (2014-2019)"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="t/giorno (2014-2019)"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="P(Bt AND Pr)" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{425A1A75-06E6-4CC9-B972-727A212EC0D3}" name="P(Bt | Pr)"/>
-    <tableColumn id="7" xr3:uid="{74CF2C72-BA58-4801-A149-31F371AAE7DA}" name="P(Pr | Bt)"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="Probabilità" dataDxfId="0">
+      <calculatedColumnFormula>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C3</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1127,8 +1341,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Tabella3" displayName="Tabella3" ref="A2:F22" totalsRowShown="0">
   <autoFilter ref="A2:F22" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="ABO" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Priorità" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="ABO" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Priorità" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="p/anno (2014-2019)">
       <calculatedColumnFormula>AVERAGE(Dati_OPTN!C3:H3)</calculatedColumnFormula>
     </tableColumn>
@@ -1468,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA86"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F74" sqref="F74"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,36 +1698,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="O1" s="35" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="O1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
+      <c r="P1" s="53"/>
+      <c r="Q1" s="53"/>
+      <c r="R1" s="53"/>
+      <c r="S1" s="53"/>
+      <c r="T1" s="53"/>
+      <c r="U1" s="53"/>
+      <c r="V1" s="53"/>
+      <c r="W1" s="53"/>
+      <c r="X1" s="53"/>
+      <c r="Y1" s="53"/>
+      <c r="Z1" s="53"/>
+      <c r="AA1" s="53"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -2933,36 +3147,36 @@
       <c r="M23" s="3"/>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
+      <c r="A24" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="35"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="O24" s="35" t="s">
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
+      <c r="M24" s="53"/>
+      <c r="O24" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="35"/>
-      <c r="S24" s="35"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
-      <c r="X24" s="35"/>
-      <c r="Y24" s="35"/>
-      <c r="Z24" s="35"/>
-      <c r="AA24" s="35"/>
+      <c r="P24" s="53"/>
+      <c r="Q24" s="53"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="53"/>
+      <c r="T24" s="53"/>
+      <c r="U24" s="53"/>
+      <c r="V24" s="53"/>
+      <c r="W24" s="53"/>
+      <c r="X24" s="53"/>
+      <c r="Y24" s="53"/>
+      <c r="Z24" s="53"/>
+      <c r="AA24" s="53"/>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -4555,36 +4769,36 @@
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="36"/>
-      <c r="O47" s="35" t="s">
+      <c r="B47" s="54"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="54"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="54"/>
+      <c r="O47" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="P47" s="35"/>
-      <c r="Q47" s="35"/>
-      <c r="R47" s="35"/>
-      <c r="S47" s="35"/>
-      <c r="T47" s="35"/>
-      <c r="U47" s="35"/>
-      <c r="V47" s="35"/>
-      <c r="W47" s="35"/>
-      <c r="X47" s="35"/>
-      <c r="Y47" s="35"/>
-      <c r="Z47" s="35"/>
-      <c r="AA47" s="35"/>
+      <c r="P47" s="53"/>
+      <c r="Q47" s="53"/>
+      <c r="R47" s="53"/>
+      <c r="S47" s="53"/>
+      <c r="T47" s="53"/>
+      <c r="U47" s="53"/>
+      <c r="V47" s="53"/>
+      <c r="W47" s="53"/>
+      <c r="X47" s="53"/>
+      <c r="Y47" s="53"/>
+      <c r="Z47" s="53"/>
+      <c r="AA47" s="53"/>
     </row>
     <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -6397,13 +6611,13 @@
       </c>
     </row>
     <row r="70" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A70" s="34" t="s">
+      <c r="A70" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="B70" s="34"/>
-      <c r="C70" s="34"/>
-      <c r="D70" s="34"/>
-      <c r="E70" s="34"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="52"/>
+      <c r="E70" s="52"/>
     </row>
     <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -6690,8 +6904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:B27"/>
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6705,14 +6919,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -7189,14 +7403,14 @@
       <c r="B23" s="1"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="41"/>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="42"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="60"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -7566,8 +7780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7586,16 +7800,16 @@
     <col min="14" max="14" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -7609,16 +7823,10 @@
         <v>48</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -7634,19 +7842,11 @@
         <v>12.105479452054794</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E3:E22" si="0">C3/$C$3</f>
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/$C3</f>
-        <v>1</v>
-      </c>
-      <c r="G3" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>0.1193667631710469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -7660,19 +7860,11 @@
         <v>3.6529680365296802E-3</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="0"/>
-        <v>3.0176153294858739E-4</v>
-      </c>
-      <c r="F4" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G4" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>3.5714285714285712E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>21</v>
@@ -7686,19 +7878,11 @@
         <v>4.6054794520547944</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>0.38044585266493153</v>
-      </c>
-      <c r="F5" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G5" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>6.0025352766486739E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>23</v>
@@ -7712,19 +7896,11 @@
         <v>7.7082191780821914</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="0"/>
-        <v>0.63675455471313791</v>
-      </c>
-      <c r="F6" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G6" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>0.30088227430710274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -7740,19 +7916,11 @@
         <v>6.338356164383562</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="0"/>
-        <v>0.52359397985741762</v>
-      </c>
-      <c r="F7" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G7" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>0.12814571370543379</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>19</v>
@@ -7766,19 +7934,11 @@
         <v>2.7397260273972603E-3</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="0"/>
-        <v>2.2632114971144054E-4</v>
-      </c>
-      <c r="F8" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G8" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>5.2631578947368418E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>21</v>
@@ -7792,19 +7952,11 @@
         <v>2.5036529680365298</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="0"/>
-        <v>0.20681981064463809</v>
-      </c>
-      <c r="F9" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G9" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>6.6444498303441596E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -7818,19 +7970,11 @@
         <v>3.9470319634703199</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>0.32605333635094869</v>
-      </c>
-      <c r="F10" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G10" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>0.32265770810003735</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -7846,19 +7990,11 @@
         <v>3.4981735159817351</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="0"/>
-        <v>0.28897438798989095</v>
-      </c>
-      <c r="F11" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G11" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>0.10598619315745057</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>19</v>
@@ -7872,19 +8008,11 @@
         <v>9.1324200913242006E-4</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="0"/>
-        <v>7.5440383237146847E-5</v>
-      </c>
-      <c r="F12" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G12" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>21</v>
@@ -7898,19 +8026,11 @@
         <v>1.2205479452054795</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="0"/>
-        <v>0.10082607219644676</v>
-      </c>
-      <c r="F13" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G13" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>4.9482589459264335E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>23</v>
@@ -7924,19 +8044,11 @@
         <v>2.3237442922374427</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="0"/>
-        <v>0.19195805514692013</v>
-      </c>
-      <c r="F14" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G14" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>0.26888935855436963</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -7952,19 +8064,11 @@
         <v>1.9420091324200914</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="0"/>
-        <v>0.16042397495379276</v>
-      </c>
-      <c r="F15" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G15" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>0.12875783355030124</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>19</v>
@@ -7978,16 +8082,8 @@
         <v>0</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="0"/>
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
         <v>0</v>
-      </c>
-      <c r="F16" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G16" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
@@ -8004,16 +8100,8 @@
         <v>0.77579908675799092</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="0"/>
-        <v>6.4086605559956253E-2</v>
-      </c>
-      <c r="F17" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G17" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>#VALUE!</v>
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>6.7452755280292209E-2</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
@@ -8030,21 +8118,13 @@
         <v>1.2123287671232876</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="0"/>
-        <v>0.10014710874731243</v>
-      </c>
-      <c r="F18" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G18" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>#VALUE!</v>
-      </c>
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>0.32548731151158516</v>
+      </c>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -8062,21 +8142,13 @@
         <v>0.32694063926940636</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="0"/>
-        <v>2.7007657198898569E-2</v>
-      </c>
-      <c r="F19" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C3</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G19" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>#VALUE!</v>
-      </c>
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>8.45835794447726E-2</v>
+      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -8092,21 +8164,13 @@
         <v>0</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" si="0"/>
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
         <v>0</v>
       </c>
-      <c r="F20" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C4</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G20" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
@@ -8122,21 +8186,13 @@
         <v>0.10547945205479452</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="0"/>
-        <v>8.7133642638904611E-3</v>
-      </c>
-      <c r="F21" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C5</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G21" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>#VALUE!</v>
-      </c>
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>3.662597114317425E-2</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -8152,21 +8208,13 @@
         <v>0.22511415525114156</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="0"/>
-        <v>1.8596054467956698E-2</v>
-      </c>
-      <c r="F22" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C6</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G22" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>#VALUE!</v>
-      </c>
+        <f>Tabella5[[#This Row],[d/anno (2014-2019)]]/Tabella3[[#This Row],[p/anno (2014-2019)]]</f>
+        <v>0.22087813620071686</v>
+      </c>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -8185,13 +8233,13 @@
       <c r="O23" s="6"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43"/>
-      <c r="E24" s="43"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
@@ -8201,22 +8249,16 @@
         <v>3</v>
       </c>
       <c r="C25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="E25" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>16</v>
       </c>
@@ -8224,7 +8266,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(Dati_OPTN!Q49:V49)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q49:V49) &gt; Arrivi!C3, Arrivi!C3, AVERAGE(Dati_OPTN!Q49:V49))</f>
         <v>11046.5</v>
       </c>
       <c r="D26" s="5">
@@ -8232,16 +8274,8 @@
         <v>30.264383561643836</v>
       </c>
       <c r="E26" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>1</v>
-      </c>
-      <c r="F26" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C26</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G26" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C3</f>
+        <v>0.2984236617333868</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -8250,7 +8284,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(Dati_OPTN!Q50:V50)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q50:V50) &gt; Arrivi!C4, Arrivi!C4, AVERAGE(Dati_OPTN!Q50:V50))</f>
         <v>3.3333333333333335</v>
       </c>
       <c r="D27" s="5">
@@ -8258,16 +8292,8 @@
         <v>9.1324200913242021E-3</v>
       </c>
       <c r="E27" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>3.0175470360144241E-4</v>
-      </c>
-      <c r="F27" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C27</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G27" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C4</f>
+        <v>8.9285714285714288E-2</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -8276,7 +8302,7 @@
         <v>21</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(Dati_OPTN!Q51:V51)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q51:V51) &gt; Arrivi!C5, Arrivi!C5, AVERAGE(Dati_OPTN!Q51:V51))</f>
         <v>2905.8333333333335</v>
       </c>
       <c r="D28" s="5">
@@ -8284,16 +8310,8 @@
         <v>7.961187214611873</v>
       </c>
       <c r="E28" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>0.26305466286455742</v>
-      </c>
-      <c r="F28" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C28</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G28" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C5</f>
+        <v>0.10376185063292646</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -8302,7 +8320,7 @@
         <v>23</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(Dati_OPTN!Q52:V52)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q52:V52) &gt; Arrivi!C6, Arrivi!C6, AVERAGE(Dati_OPTN!Q52:V52))</f>
         <v>9278.6666666666661</v>
       </c>
       <c r="D29" s="5">
@@ -8310,16 +8328,8 @@
         <v>25.421004566210044</v>
       </c>
       <c r="E29" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>0.83996439294497494</v>
-      </c>
-      <c r="F29" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C29</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G29" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C6</f>
+        <v>0.99228232777827274</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
@@ -8330,7 +8340,7 @@
         <v>17</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(Dati_OPTN!Q53:V53)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q53:V53) &gt; Arrivi!C7, Arrivi!C7, AVERAGE(Dati_OPTN!Q53:V53))</f>
         <v>5731.833333333333</v>
       </c>
       <c r="D30" s="5">
@@ -8338,16 +8348,8 @@
         <v>15.703652968036529</v>
       </c>
       <c r="E30" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>0.51888230057786022</v>
-      </c>
-      <c r="F30" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C26</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G30" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C7</f>
+        <v>0.31748859880725983</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
@@ -8356,7 +8358,7 @@
         <v>19</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(Dati_OPTN!Q54:V54)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q54:V54) &gt; Arrivi!C8, Arrivi!C8, AVERAGE(Dati_OPTN!Q54:V54))</f>
         <v>2.3333333333333335</v>
       </c>
       <c r="D31" s="5">
@@ -8364,16 +8366,8 @@
         <v>6.392694063926941E-3</v>
       </c>
       <c r="E31" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>2.1122829252100968E-4</v>
-      </c>
-      <c r="F31" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C27</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G31" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C8</f>
+        <v>0.12280701754385966</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
@@ -8382,7 +8376,7 @@
         <v>21</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(Dati_OPTN!Q55:V55)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q55:V55) &gt; Arrivi!C9, Arrivi!C9, AVERAGE(Dati_OPTN!Q55:V55))</f>
         <v>1521.5</v>
       </c>
       <c r="D32" s="5">
@@ -8390,16 +8384,8 @@
         <v>4.1684931506849319</v>
       </c>
       <c r="E32" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>0.13773593445887838</v>
-      </c>
-      <c r="F32" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C28</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G32" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C9</f>
+        <v>0.11062772661173048</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -8408,24 +8394,16 @@
         <v>23</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(Dati_OPTN!Q56:V56)</f>
-        <v>4760.833333333333</v>
+        <f>IF(AVERAGE(Dati_OPTN!Q56:V56) &gt; Arrivi!C10, Arrivi!C10, AVERAGE(Dati_OPTN!Q56:V56))</f>
+        <v>4465</v>
       </c>
       <c r="D33" s="5">
         <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/365</f>
-        <v>13.043378995433789</v>
+        <v>12.232876712328768</v>
       </c>
       <c r="E33" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>0.43098115541876009</v>
-      </c>
-      <c r="F33" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C29</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G33" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C10</f>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -8436,7 +8414,7 @@
         <v>17</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(Dati_OPTN!Q57:V57)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q57:V57) &gt; Arrivi!C11, Arrivi!C11, AVERAGE(Dati_OPTN!Q57:V57))</f>
         <v>3254.1666666666665</v>
       </c>
       <c r="D34" s="5">
@@ -8444,16 +8422,8 @@
         <v>8.9155251141552512</v>
       </c>
       <c r="E34" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>0.29458802939090811</v>
-      </c>
-      <c r="F34" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C26</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G34" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C11</f>
+        <v>0.27011883845440837</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -8462,7 +8432,7 @@
         <v>19</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(Dati_OPTN!Q58:V58)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q58:V58) &gt; Arrivi!C12, Arrivi!C12, AVERAGE(Dati_OPTN!Q58:V58))</f>
         <v>0.5</v>
       </c>
       <c r="D35" s="5">
@@ -8470,16 +8440,8 @@
         <v>1.3698630136986301E-3</v>
       </c>
       <c r="E35" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>4.5263205540216361E-5</v>
-      </c>
-      <c r="F35" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C27</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G35" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C12</f>
+        <v>4.6875E-2</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -8488,7 +8450,7 @@
         <v>21</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(Dati_OPTN!Q59:V59)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q59:V59) &gt; Arrivi!C13, Arrivi!C13, AVERAGE(Dati_OPTN!Q59:V59))</f>
         <v>853.33333333333337</v>
       </c>
       <c r="D36" s="5">
@@ -8496,16 +8458,8 @@
         <v>2.3378995433789957</v>
       </c>
       <c r="E36" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>7.7249204121969256E-2</v>
-      </c>
-      <c r="F36" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C28</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G36" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C13</f>
+        <v>9.4781465780558696E-2</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -8514,7 +8468,7 @@
         <v>23</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(Dati_OPTN!Q60:V60)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q60:V60) &gt; Arrivi!C14, Arrivi!C14, AVERAGE(Dati_OPTN!Q60:V60))</f>
         <v>2782.5</v>
       </c>
       <c r="D37" s="5">
@@ -8522,16 +8476,8 @@
         <v>7.6232876712328768</v>
       </c>
       <c r="E37" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>0.25188973883130406</v>
-      </c>
-      <c r="F37" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C29</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G37" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C14</f>
+        <v>0.88211983514741621</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -8542,7 +8488,7 @@
         <v>17</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(Dati_OPTN!Q61:V61)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q61:V61) &gt; Arrivi!C15, Arrivi!C15, AVERAGE(Dati_OPTN!Q61:V61))</f>
         <v>1750.8333333333333</v>
       </c>
       <c r="D38" s="5">
@@ -8550,16 +8496,8 @@
         <v>4.7968036529680367</v>
       </c>
       <c r="E38" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>0.15849665806665761</v>
-      </c>
-      <c r="F38" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C26</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G38" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C15</f>
+        <v>0.31803457358239229</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -8568,7 +8506,7 @@
         <v>19</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(Dati_OPTN!Q62:V62)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q62:V62) &gt; Arrivi!C16, Arrivi!C16, AVERAGE(Dati_OPTN!Q62:V62))</f>
         <v>0</v>
       </c>
       <c r="D39" s="5">
@@ -8576,16 +8514,8 @@
         <v>0</v>
       </c>
       <c r="E39" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C16</f>
         <v>0</v>
-      </c>
-      <c r="F39" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C27</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G39" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>#VALUE!</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -8594,7 +8524,7 @@
         <v>21</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(Dati_OPTN!Q63:V63)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q63:V63) &gt; Arrivi!C17, Arrivi!C17, AVERAGE(Dati_OPTN!Q63:V63))</f>
         <v>454</v>
       </c>
       <c r="D40" s="5">
@@ -8602,16 +8532,8 @@
         <v>1.2438356164383562</v>
       </c>
       <c r="E40" s="5">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>4.1098990630516453E-2</v>
-      </c>
-      <c r="F40" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C28</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G40" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>#VALUE!</v>
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C17</f>
+        <v>0.1081467365412101</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -8620,24 +8542,16 @@
         <v>23</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(Dati_OPTN!Q64:V64)</f>
-        <v>1459.6666666666667</v>
+        <f>IF(AVERAGE(Dati_OPTN!Q64:V64) &gt; Arrivi!C18, Arrivi!C18, AVERAGE(Dati_OPTN!Q64:V64))</f>
+        <v>1359.5</v>
       </c>
       <c r="D41" s="5">
         <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/365</f>
-        <v>3.999086757990868</v>
-      </c>
-      <c r="E41" s="6">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>0.13213838470707162</v>
-      </c>
-      <c r="F41" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C29</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G41" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>#VALUE!</v>
+        <v>3.7246575342465755</v>
+      </c>
+      <c r="E41" s="5">
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C18</f>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -8648,24 +8562,16 @@
         <v>17</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(Dati_OPTN!Q65:V65)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q65:V65) &gt; Arrivi!C19, Arrivi!C19, AVERAGE(Dati_OPTN!Q65:V65))</f>
         <v>309.83333333333331</v>
       </c>
       <c r="D42" s="5">
         <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/365</f>
         <v>0.84885844748858441</v>
       </c>
-      <c r="E42" s="6">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>2.8048099699754067E-2</v>
-      </c>
-      <c r="F42" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C26</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G42" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>#VALUE!</v>
+      <c r="E42" s="5">
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C19</f>
+        <v>0.21961015948021265</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -8674,24 +8580,16 @@
         <v>19</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(Dati_OPTN!Q66:V66)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q66:V66) &gt; Arrivi!C20, Arrivi!C20, AVERAGE(Dati_OPTN!Q66:V66))</f>
         <v>0.5</v>
       </c>
       <c r="D43" s="5">
         <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/365</f>
         <v>1.3698630136986301E-3</v>
       </c>
-      <c r="E43" s="6">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>4.5263205540216361E-5</v>
-      </c>
-      <c r="F43" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C27</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G43" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>#VALUE!</v>
+      <c r="E43" s="5">
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C20</f>
+        <v>0.3</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -8700,24 +8598,16 @@
         <v>21</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(Dati_OPTN!Q67:V67)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q67:V67) &gt; Arrivi!C21, Arrivi!C21, AVERAGE(Dati_OPTN!Q67:V67))</f>
         <v>77</v>
       </c>
       <c r="D44" s="5">
         <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/365</f>
         <v>0.21095890410958903</v>
       </c>
-      <c r="E44" s="6">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>6.970533653193319E-3</v>
-      </c>
-      <c r="F44" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C28</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G44" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>#VALUE!</v>
+      <c r="E44" s="5">
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C21</f>
+        <v>7.3251942286348501E-2</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -8726,24 +8616,16 @@
         <v>23</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(Dati_OPTN!Q68:V68)</f>
+        <f>IF(AVERAGE(Dati_OPTN!Q68:V68) &gt; Arrivi!C22, Arrivi!C22, AVERAGE(Dati_OPTN!Q68:V68))</f>
         <v>275.83333333333331</v>
       </c>
       <c r="D45" s="5">
         <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/365</f>
         <v>0.75570776255707761</v>
       </c>
-      <c r="E45" s="6">
-        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/$C$26</f>
-        <v>2.4970201723019357E-2</v>
-      </c>
-      <c r="F45" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C29</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G45" t="e">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>#VALUE!</v>
+      <c r="E45" s="5">
+        <f>Tabella511[[#This Row],[r/anno (2014-2019)]]/Arrivi!C22</f>
+        <v>0.74148745519713255</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -8770,6 +8652,7 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
@@ -8781,17 +8664,18 @@
       <c r="Q47" s="6"/>
     </row>
     <row r="48" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="46"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="62" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="63"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>2</v>
       </c>
@@ -8799,22 +8683,19 @@
         <v>3</v>
       </c>
       <c r="C49" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D49" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D49" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="E49" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G49" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
@@ -8830,19 +8711,11 @@
         <v>54.092694063926935</v>
       </c>
       <c r="E50" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>1</v>
-      </c>
-      <c r="F50">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C50</f>
-        <v>1</v>
-      </c>
-      <c r="G50">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C3</f>
+        <v>0.53338406191889132</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
         <v>19</v>
@@ -8856,19 +8729,11 @@
         <v>4.5205479452054796E-2</v>
       </c>
       <c r="E51" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>8.3570397508082699E-4</v>
-      </c>
-      <c r="F51">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C51</f>
-        <v>1</v>
-      </c>
-      <c r="G51">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>8.3570397508082699E-4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C4</f>
+        <v>0.4419642857142857</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
         <v>21</v>
@@ -8882,19 +8747,11 @@
         <v>49.414155251141558</v>
       </c>
       <c r="E52" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>0.91350885930628145</v>
-      </c>
-      <c r="F52">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C52</f>
-        <v>1</v>
-      </c>
-      <c r="G52">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>0.91350885930628145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C5</f>
+        <v>0.64403763636039024</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1" t="s">
         <v>23</v>
@@ -8908,19 +8765,11 @@
         <v>4.2356164383561641</v>
       </c>
       <c r="E53" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>7.830293002878537E-2</v>
-      </c>
-      <c r="F53">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C53</f>
-        <v>1</v>
-      </c>
-      <c r="G53">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>7.830293002878537E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C6</f>
+        <v>0.1653328580340433</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>24</v>
       </c>
@@ -8936,19 +8785,11 @@
         <v>24.426027397260274</v>
       </c>
       <c r="E54" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>0.45155871453534019</v>
-      </c>
-      <c r="F54">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C50</f>
-        <v>0.45155871453534019</v>
-      </c>
-      <c r="G54">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C7</f>
+        <v>0.49383320101179812</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1" t="s">
         <v>19</v>
@@ -8962,19 +8803,11 @@
         <v>2.0547945205479451E-2</v>
       </c>
       <c r="E55" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>3.7986544321855773E-4</v>
-      </c>
-      <c r="F55">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C51</f>
-        <v>0.45454545454545453</v>
-      </c>
-      <c r="G55">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>8.4123156300824409E-4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C8</f>
+        <v>0.39473684210526316</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1" t="s">
         <v>21</v>
@@ -8988,19 +8821,11 @@
         <v>22.43013698630137</v>
       </c>
       <c r="E56" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>0.41466111781737758</v>
-      </c>
-      <c r="F56">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C52</f>
-        <v>0.45392128778288066</v>
-      </c>
-      <c r="G56">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>0.91828837417979925</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C9</f>
+        <v>0.59527387300048473</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1" t="s">
         <v>23</v>
@@ -9014,19 +8839,11 @@
         <v>1.800456621004566</v>
       </c>
       <c r="E57" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>3.3284654280239398E-2</v>
-      </c>
-      <c r="F57">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C53</f>
-        <v>0.42507546356188008</v>
-      </c>
-      <c r="G57">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$54</f>
-        <v>7.3710578954255687E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C10</f>
+        <v>0.14718178424785366</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>25</v>
       </c>
@@ -9042,19 +8859,11 @@
         <v>19.62283105022831</v>
       </c>
       <c r="E58" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>0.36276305681942883</v>
-      </c>
-      <c r="F58">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C50</f>
-        <v>0.36276305681942883</v>
-      </c>
-      <c r="G58">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C11</f>
+        <v>0.59452430031957726</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
         <v>19</v>
@@ -9068,19 +8877,11 @@
         <v>1.187214611872146E-2</v>
       </c>
       <c r="E59" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>2.1947781163738888E-4</v>
-      </c>
-      <c r="F59">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C51</f>
-        <v>0.2626262626262626</v>
-      </c>
-      <c r="G59">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>6.0501698701540462E-4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C12</f>
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
         <v>21</v>
@@ -9094,19 +8895,11 @@
         <v>17.739726027397261</v>
       </c>
       <c r="E60" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>0.32795049931202147</v>
-      </c>
-      <c r="F60">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C52</f>
-        <v>0.35900089634715432</v>
-      </c>
-      <c r="G60">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>0.90403499790571051</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C13</f>
+        <v>0.71919139562005963</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
         <v>23</v>
@@ -9120,19 +8913,11 @@
         <v>1.7132420091324201</v>
       </c>
       <c r="E61" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>3.1672336510133972E-2</v>
-      </c>
-      <c r="F61">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C53</f>
-        <v>0.40448469167744722</v>
-      </c>
-      <c r="G61">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$58</f>
-        <v>8.7308605203146095E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C14</f>
+        <v>0.19824579942935644</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>26</v>
       </c>
@@ -9148,19 +8933,11 @@
         <v>7.3986301369863012</v>
       </c>
       <c r="E62" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>0.13677688392156201</v>
-      </c>
-      <c r="F62">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C50</f>
-        <v>0.13677688392156201</v>
-      </c>
-      <c r="G62">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C15</f>
+        <v>0.49053919045744904</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
         <v>19</v>
@@ -9174,19 +8951,11 @@
         <v>1.0502283105022832E-2</v>
       </c>
       <c r="E63" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>1.9415344875615173E-4</v>
-      </c>
-      <c r="F63">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C51</f>
-        <v>0.23232323232323232</v>
-      </c>
-      <c r="G63">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>1.4194902178608899E-3</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C16</f>
+        <v>0.63888888888888895</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
         <v>21</v>
@@ -9200,19 +8969,11 @@
         <v>6.7986301369863016</v>
       </c>
       <c r="E64" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>0.12568481297958012</v>
-      </c>
-      <c r="F64">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C52</f>
-        <v>0.1375846678433148</v>
-      </c>
-      <c r="G64">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>0.91890390668394739</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C17</f>
+        <v>0.59111481657932352</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
         <v>23</v>
@@ -9226,19 +8987,11 @@
         <v>0.54292237442922375</v>
       </c>
       <c r="E65" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>1.0036889155263668E-2</v>
-      </c>
-      <c r="F65">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C53</f>
-        <v>0.12818025010780509</v>
-      </c>
-      <c r="G65">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$62</f>
-        <v>7.3381472566808617E-2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C18</f>
+        <v>0.14576437415716562</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>27</v>
       </c>
@@ -9254,19 +9007,11 @@
         <v>2.6452054794520548</v>
       </c>
       <c r="E66" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>4.8901344723668999E-2</v>
-      </c>
-      <c r="F66">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C50</f>
-        <v>4.8901344723668999E-2</v>
-      </c>
-      <c r="G66">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C19</f>
+        <v>0.68434731246308333</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
         <v>19</v>
@@ -9280,19 +9025,11 @@
         <v>2.2831050228310505E-3</v>
       </c>
       <c r="E67" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>4.2207271468728638E-5</v>
-      </c>
-      <c r="F67">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C51</f>
-        <v>5.0505050505050504E-2</v>
-      </c>
-      <c r="G67">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>8.6311065078543069E-4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C20</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
         <v>21</v>
@@ -9306,19 +9043,11 @@
         <v>2.4456621004566208</v>
       </c>
       <c r="E68" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>4.5212429197302111E-2</v>
-      </c>
-      <c r="F68">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C52</f>
-        <v>4.9493148026650148E-2</v>
-      </c>
-      <c r="G68">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>0.92456412912135333</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C21</f>
+        <v>0.84921515776121759</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
         <v>23</v>
@@ -9332,24 +9061,17 @@
         <v>0.17899543378995433</v>
       </c>
       <c r="E69" s="6">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$50</f>
-        <v>3.3090500831483246E-3</v>
-      </c>
-      <c r="F69">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C53</f>
-        <v>4.2259594652867612E-2</v>
-      </c>
-      <c r="G69">
-        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/$C$66</f>
-        <v>6.7667875021577756E-2</v>
+        <f>Tabella512[[#This Row],[t/anno (2014-2019)]]/Arrivi!C22</f>
+        <v>0.17562724014336917</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A48:E48"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="3">
@@ -9362,10 +9084,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9385,61 +9107,61 @@
     <col min="16" max="16" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49" t="s">
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="L2" s="68"/>
+      <c r="M2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="L2" s="50"/>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -9447,16 +9169,16 @@
         <v>3</v>
       </c>
       <c r="C3" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>67</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>2</v>
@@ -9465,21 +9187,21 @@
         <v>42</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="L3" s="15" t="s">
         <v>69</v>
-      </c>
-      <c r="L3" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="M3" s="13"/>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>24</v>
       </c>
@@ -9495,54 +9217,50 @@
       <c r="E4" s="18">
         <v>6.392694063926941E-3</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <f>C4*(1-Uscite!E8-Uscite!E31)</f>
-        <v>5.2032017974239959E-2</v>
+        <v>4.2922374429223746E-2</v>
       </c>
       <c r="G4" s="19" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I4" s="18">
         <v>22.411872146118721</v>
       </c>
       <c r="J4" s="21">
         <f>1/(I$4+SUM(F$4:F$6))</f>
-        <v>1.9946762001335716E-2</v>
+        <v>2.0195499815566207E-2</v>
       </c>
       <c r="K4" s="22">
-        <f t="shared" ref="K4:K15" si="0">F4*J4</f>
-        <v>1.0378702789813866E-3</v>
+        <f>F4*J4</f>
+        <v>8.6683880486905182E-4</v>
       </c>
       <c r="L4" s="22">
         <f>SUM(K$4:K$6)</f>
-        <v>0.55295572029700468</v>
+        <v>0.54738104020656575</v>
       </c>
       <c r="M4" s="21">
         <f>IF(MOD(ROW(),3)=1,(L4*J4)/(1-K4),IF(MOD(ROW(),3)=2,(L4*J4)/((1-K4)*(1-K4-K5)), IF(MOD(ROW(),3)=0,(L4*J4)/((1-K4-K5)*(1-L4)))))</f>
-        <v>1.1041135416336339E-2</v>
+        <v>1.106422459576153E-2</v>
       </c>
       <c r="N4" s="21">
-        <f t="shared" ref="N4:N15" si="1">M4+J4</f>
-        <v>3.0987897417672057E-2</v>
+        <f t="shared" ref="N4:N15" si="0">M4+J4</f>
+        <v>3.1259724411327738E-2</v>
       </c>
       <c r="O4" s="21">
-        <f t="shared" ref="O4:O15" si="2">M4*F4</f>
-        <v>5.7449255643882982E-4</v>
+        <f t="shared" ref="O4:O5" si="1">M4*F4</f>
+        <v>4.7490279086830311E-4</v>
       </c>
       <c r="P4" s="21">
-        <f t="shared" ref="P4:P15" si="3">N4*F4</f>
-        <v>1.6123628354202165E-3</v>
-      </c>
-      <c r="Q4" s="23">
-        <f t="shared" ref="Q4:Q15" si="4">(D4/E4)</f>
-        <v>0.42857142857142855</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
+        <f t="shared" ref="P4:P5" si="2">N4*F4</f>
+        <v>1.3417415957373551E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
       <c r="B5" s="17" t="s">
         <v>21</v>
       </c>
@@ -9555,52 +9273,48 @@
       <c r="E5" s="18">
         <v>4.1684931506849319</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <f>C5*(1-Uscite!E9-Uscite!E32)</f>
-        <v>24.697378956190793</v>
+        <v>31.008219178082197</v>
       </c>
       <c r="G5" s="19"/>
       <c r="H5" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I5" s="18">
         <v>12.106849315068493</v>
       </c>
       <c r="J5" s="21">
         <f>J4</f>
-        <v>1.9946762001335716E-2</v>
+        <v>2.0195499815566207E-2</v>
       </c>
       <c r="K5" s="22">
-        <f t="shared" si="0"/>
-        <v>0.49263274009593488</v>
+        <f t="shared" ref="K5" si="3">F5*J5</f>
+        <v>0.62622648469199549</v>
       </c>
       <c r="L5" s="22">
         <f>L4</f>
-        <v>0.55295572029700468</v>
+        <v>0.54738104020656575</v>
       </c>
       <c r="M5" s="21">
         <f>IF(MOD(ROW(),3)=1,(L4*J4)/(1-K4),IF(MOD(ROW(),3)=2,(L4*J4)/((1-K4)*(1-K4-K5)), IF(MOD(ROW(),3)=0,(L4*J4)/((1-K4-K5)*(1-L4)))))</f>
-        <v>2.1806230573563679E-2</v>
+        <v>2.9670223927107671E-2</v>
       </c>
       <c r="N5" s="21">
+        <f t="shared" si="0"/>
+        <v>4.9865723742673881E-2</v>
+      </c>
+      <c r="O5" s="21">
         <f t="shared" si="1"/>
-        <v>4.1752992574899395E-2</v>
-      </c>
-      <c r="O5" s="21">
+        <v>0.92002080659453334</v>
+      </c>
+      <c r="P5" s="21">
         <f t="shared" si="2"/>
-        <v>0.53855674008137588</v>
-      </c>
-      <c r="P5" s="21">
-        <f t="shared" si="3"/>
-        <v>1.0311894801773107</v>
-      </c>
-      <c r="Q5" s="23">
-        <f t="shared" si="4"/>
-        <v>0.60061342972943366</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
+        <v>1.546247291286529</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
       <c r="B6" s="17" t="s">
         <v>23</v>
       </c>
@@ -9613,51 +9327,47 @@
       <c r="E6" s="18">
         <v>13.043378995433789</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="32">
         <f>C6*(1-Uscite!E10-Uscite!E33)</f>
-        <v>2.9721671075294531</v>
+        <v>-3.9470319634703199</v>
       </c>
       <c r="G6" s="19"/>
       <c r="H6" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I6" s="18">
         <v>10.305022831050229</v>
       </c>
       <c r="J6" s="21">
         <f>J5</f>
-        <v>1.9946762001335716E-2</v>
+        <v>2.0195499815566207E-2</v>
       </c>
       <c r="K6" s="22">
-        <f t="shared" si="0"/>
-        <v>5.928510992208838E-2</v>
+        <f>F6*J6</f>
+        <v>-7.9712283290298766E-2</v>
       </c>
       <c r="L6" s="22">
         <f>L5</f>
-        <v>0.55295572029700468</v>
+        <v>0.54738104020656575</v>
       </c>
       <c r="M6" s="21">
         <f>IF(MOD(ROW(),3)=1,(L4*J4)/(1-K4),IF(MOD(ROW(),3)=2,(L4*J4)/((1-K4)*(1-K4-K5)), IF(MOD(ROW(),3)=0,(L4*J4)/((1-K4-K5)*(1-L4)))))</f>
-        <v>4.8728055640097266E-2</v>
+        <v>6.5495498993651591E-2</v>
       </c>
       <c r="N6" s="21">
-        <f t="shared" si="1"/>
-        <v>6.8674817641432989E-2</v>
+        <f t="shared" si="0"/>
+        <v>8.5690998809217794E-2</v>
       </c>
       <c r="O6" s="21">
-        <f t="shared" si="2"/>
-        <v>0.14482792418736215</v>
+        <f>M6*F6</f>
+        <v>-0.25851282799138098</v>
       </c>
       <c r="P6" s="21">
-        <f t="shared" si="3"/>
-        <v>0.20411303410945056</v>
-      </c>
-      <c r="Q6" s="23">
-        <f t="shared" si="4"/>
-        <v>0.30260808681953444</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <f>N6*F6</f>
+        <v>-0.33822511128167976</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>25</v>
       </c>
@@ -9673,54 +9383,50 @@
       <c r="E7" s="18">
         <v>1.3698630136986301E-3</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <f>C7*(1-Uscite!E12-Uscite!E35)</f>
-        <v>2.9220216881423858E-2</v>
+        <v>2.6940639269406392E-2</v>
       </c>
       <c r="G7" s="19" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I7" s="18">
         <v>13.938356164383562</v>
       </c>
       <c r="J7" s="21">
         <f>1/(I$7+SUM(F7:F9))</f>
-        <v>2.5609757636762279E-2</v>
+        <v>2.9613803548247511E-2</v>
       </c>
       <c r="K7" s="22">
-        <f t="shared" si="0"/>
-        <v>7.4832267242689471E-4</v>
+        <f>F7*J7</f>
+        <v>7.9781479878840325E-4</v>
       </c>
       <c r="L7" s="22">
         <f>SUM(K$7:K$9)</f>
-        <v>0.64304207677526548</v>
+        <v>0.58723225876244034</v>
       </c>
       <c r="M7" s="21">
         <f>IF(MOD(ROW(),3)=1,(L7*J7)/(1-K7),IF(MOD(ROW(),3)=2,(L7*J7)/((1-K7)*(1-K7-K8)), IF(MOD(ROW(),3)=0,(L7*J7)/((1-K7-K8)*(1-L7)))))</f>
-        <v>1.6480484456626303E-2</v>
+        <v>1.7404065969574174E-2</v>
       </c>
       <c r="N7" s="21">
-        <f t="shared" si="1"/>
-        <v>4.2090242093388582E-2</v>
+        <f t="shared" si="0"/>
+        <v>4.7017869517821685E-2</v>
       </c>
       <c r="O7" s="21">
-        <f t="shared" si="2"/>
-        <v>4.8156333013355538E-4</v>
+        <f>M7*F7</f>
+        <v>4.6887666310724941E-4</v>
       </c>
       <c r="P7" s="21">
-        <f t="shared" si="3"/>
-        <v>1.22988600256045E-3</v>
-      </c>
-      <c r="Q7" s="23">
-        <f t="shared" si="4"/>
-        <v>0.66666666666666663</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="24"/>
+        <f>N7*F7</f>
+        <v>1.2666914618956527E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
       <c r="B8" s="17" t="s">
         <v>21</v>
       </c>
@@ -9733,52 +9439,48 @@
       <c r="E8" s="18">
         <v>2.3378995433789957</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <f>C8*(1-Uscite!E13-Uscite!E36)</f>
-        <v>20.27376787605273</v>
+        <v>21.107762557077624</v>
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I8" s="18">
         <v>9.3986301369863021</v>
       </c>
       <c r="J8" s="21">
         <f>J7</f>
-        <v>2.5609757636762279E-2</v>
+        <v>2.9613803548247511E-2</v>
       </c>
       <c r="K8" s="22">
-        <f t="shared" si="0"/>
-        <v>0.51920628168968719</v>
+        <f>F8*J8</f>
+        <v>0.62508113370835128</v>
       </c>
       <c r="L8" s="22">
         <f>L7</f>
-        <v>0.64304207677526548</v>
+        <v>0.58723225876244034</v>
       </c>
       <c r="M8" s="21">
         <f>IF(MOD(ROW(),3)=1,(L7*J7)/(1-K7),IF(MOD(ROW(),3)=2,(L7*J7)/((1-K7)*(1-K7-K8)), IF(MOD(ROW(),3)=0,(L7*J7)/((1-K7-K8)*(1-L7)))))</f>
-        <v>3.4331095780487549E-2</v>
+        <v>4.6519878793578953E-2</v>
       </c>
       <c r="N8" s="21">
-        <f t="shared" si="1"/>
-        <v>5.9940853417249827E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.6133682341826464E-2</v>
       </c>
       <c r="O8" s="21">
-        <f t="shared" si="2"/>
-        <v>0.69602066678413788</v>
+        <f>M8*F8</f>
+        <v>0.98193055575889521</v>
       </c>
       <c r="P8" s="21">
-        <f t="shared" si="3"/>
-        <v>1.2152269484738252</v>
-      </c>
-      <c r="Q8" s="23">
-        <f t="shared" si="4"/>
-        <v>0.52207031249999991</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
+        <f>N8*F8</f>
+        <v>1.6070116894672466</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
       <c r="B9" s="17" t="s">
         <v>23</v>
       </c>
@@ -9791,51 +9493,47 @@
       <c r="E9" s="18">
         <v>7.6232876712328768</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <f>C9*(1-Uscite!E14-Uscite!E37)</f>
-        <v>4.806272443455768</v>
+        <v>-1.3050228310502283</v>
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I9" s="18">
         <v>4.5397260273972604</v>
       </c>
       <c r="J9" s="21">
         <f>J8</f>
-        <v>2.5609757636762279E-2</v>
+        <v>2.9613803548247511E-2</v>
       </c>
       <c r="K9" s="22">
-        <f t="shared" si="0"/>
-        <v>0.12308747241315145</v>
+        <f>F9*J9</f>
+        <v>-3.8646689744699265E-2</v>
       </c>
       <c r="L9" s="22">
         <f>L8</f>
-        <v>0.64304207677526548</v>
+        <v>0.58723225876244034</v>
       </c>
       <c r="M9" s="21">
         <f>IF(MOD(ROW(),3)=1,(L7*J7)/(1-K7),IF(MOD(ROW(),3)=2,(L7*J7)/((1-K7)*(1-K7-K8)), IF(MOD(ROW(),3)=0,(L7*J7)/((1-K7-K8)*(1-L7)))))</f>
-        <v>9.6104898676104361E-2</v>
+        <v>0.1126123965174096</v>
       </c>
       <c r="N9" s="21">
-        <f t="shared" si="1"/>
-        <v>0.12171465631286664</v>
+        <f t="shared" si="0"/>
+        <v>0.14222620006565712</v>
       </c>
       <c r="O9" s="21">
-        <f t="shared" si="2"/>
-        <v>0.46190632618806909</v>
+        <f>M9*F9</f>
+        <v>-0.14696174851450075</v>
       </c>
       <c r="P9" s="21">
-        <f t="shared" si="3"/>
-        <v>0.58499379860122058</v>
-      </c>
-      <c r="Q9" s="23">
-        <f t="shared" si="4"/>
-        <v>0.30482180293501043</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <f>N9*F9</f>
+        <v>-0.18560843825920001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>26</v>
       </c>
@@ -9851,7 +9549,7 @@
       <c r="E10" s="18">
         <v>0</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <f>C10*(1-Uscite!E16-Uscite!E39)</f>
         <v>1.643835616438356E-2</v>
       </c>
@@ -9859,46 +9557,42 @@
         <v>26</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I10" s="18">
         <v>4.3242009132420085</v>
       </c>
       <c r="J10" s="21">
         <f>1/(I$10+SUM(F10:F12))</f>
-        <v>5.7169957965793758E-2</v>
+        <v>7.9301853997682498E-2</v>
       </c>
       <c r="K10" s="22">
-        <f t="shared" si="0"/>
-        <v>9.3978013094455487E-4</v>
+        <f>F10*J10</f>
+        <v>1.3035921205098492E-3</v>
       </c>
       <c r="L10" s="22">
         <f>SUM(K$10:K$12)</f>
-        <v>0.75278561555430723</v>
+        <v>0.65708285052143689</v>
       </c>
       <c r="M10" s="21">
         <f>IF(MOD(ROW(),3)=1,(L10*J10)/(1-K10),IF(MOD(ROW(),3)=2,(L10*J10)/((1-K10)*(1-K10-K11)), IF(MOD(ROW(),3)=0,(L10*J10)/((1-K10-K11)*(1-L10)))))</f>
-        <v>4.3077205099943477E-2</v>
+        <v>5.2175904374254775E-2</v>
       </c>
       <c r="N10" s="21">
-        <f t="shared" si="1"/>
-        <v>0.10024716306573724</v>
+        <f t="shared" si="0"/>
+        <v>0.13147775837193726</v>
       </c>
       <c r="O10" s="21">
-        <f t="shared" si="2"/>
-        <v>7.081184399990708E-4</v>
+        <f>M10*F10</f>
+        <v>8.5768609930281811E-4</v>
       </c>
       <c r="P10" s="21">
-        <f t="shared" si="3"/>
-        <v>1.6478985709436256E-3</v>
-      </c>
-      <c r="Q10" s="23" t="e">
-        <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+        <f>N10*F10</f>
+        <v>2.1612782198126672E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
       <c r="B11" s="17" t="s">
         <v>21</v>
       </c>
@@ -9911,52 +9605,48 @@
       <c r="E11" s="18">
         <v>1.2438356164383562</v>
       </c>
-      <c r="F11" s="33">
+      <c r="F11" s="32">
         <f>C11*(1-Uscite!E17-Uscite!E40)</f>
-        <v>10.291591416965467</v>
+        <v>9.4817351598173527</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I11" s="18">
         <v>2.9876712328767123</v>
       </c>
       <c r="J11" s="21">
         <f>J10</f>
-        <v>5.7169957965793758E-2</v>
+        <v>7.9301853997682498E-2</v>
       </c>
       <c r="K11" s="22">
-        <f t="shared" si="0"/>
-        <v>0.58836984870903952</v>
+        <f>F11*J11</f>
+        <v>0.75191917728852842</v>
       </c>
       <c r="L11" s="22">
         <f>L10</f>
-        <v>0.75278561555430723</v>
+        <v>0.65708285052143689</v>
       </c>
       <c r="M11" s="21">
         <f>IF(MOD(ROW(),3)=1,(L10*J10)/(1-K10),IF(MOD(ROW(),3)=2,(L10*J10)/((1-K10)*(1-K10-K11)), IF(MOD(ROW(),3)=0,(L10*J10)/((1-K10-K11)*(1-L10)))))</f>
-        <v>0.10488973719610156</v>
+        <v>0.21142916730732506</v>
       </c>
       <c r="N11" s="21">
-        <f t="shared" si="1"/>
-        <v>0.16205969516189533</v>
+        <f t="shared" si="0"/>
+        <v>0.29073102130500755</v>
       </c>
       <c r="O11" s="21">
-        <f t="shared" si="2"/>
-        <v>1.0794823190551623</v>
+        <f>M11*F11</f>
+        <v>2.0047153694687694</v>
       </c>
       <c r="P11" s="21">
-        <f t="shared" si="3"/>
-        <v>1.667852167764202</v>
-      </c>
-      <c r="Q11" s="23">
-        <f t="shared" si="4"/>
-        <v>0.62371512481644642</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
+        <f>N11*F11</f>
+        <v>2.7566345467572981</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="23"/>
       <c r="B12" s="17" t="s">
         <v>23</v>
       </c>
@@ -9969,51 +9659,47 @@
       <c r="E12" s="18">
         <v>3.999086757990868</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="32">
         <f>C12*(1-Uscite!E18-Uscite!E41)</f>
-        <v>2.8594736209555203</v>
+        <v>-1.2123287671232879</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I12" s="18">
         <v>1.3365296803652968</v>
       </c>
       <c r="J12" s="21">
         <f>J11</f>
-        <v>5.7169957965793758E-2</v>
+        <v>7.9301853997682498E-2</v>
       </c>
       <c r="K12" s="22">
-        <f t="shared" si="0"/>
-        <v>0.16347598671432317</v>
+        <f>F12*J12</f>
+        <v>-9.61399188876014E-2</v>
       </c>
       <c r="L12" s="22">
         <f>L11</f>
-        <v>0.75278561555430723</v>
+        <v>0.65708285052143689</v>
       </c>
       <c r="M12" s="21">
         <f>IF(MOD(ROW(),3)=1,(L10*J10)/(1-K10),IF(MOD(ROW(),3)=2,(L10*J10)/((1-K10)*(1-K10-K11)), IF(MOD(ROW(),3)=0,(L10*J10)/((1-K10-K11)*(1-L10)))))</f>
-        <v>0.4238878095225273</v>
+        <v>0.6157567512498443</v>
       </c>
       <c r="N12" s="21">
-        <f t="shared" si="1"/>
-        <v>0.48105776748832108</v>
+        <f t="shared" si="0"/>
+        <v>0.69505860524752683</v>
       </c>
       <c r="O12" s="21">
-        <f t="shared" si="2"/>
-        <v>1.212096009574285</v>
+        <f>M12*F12</f>
+        <v>-0.74649962309056483</v>
       </c>
       <c r="P12" s="21">
-        <f t="shared" si="3"/>
-        <v>1.3755719962886082</v>
-      </c>
-      <c r="Q12" s="23">
-        <f t="shared" si="4"/>
-        <v>0.30315140443023519</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <f>N12*F12</f>
+        <v>-0.84263954197816626</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>27</v>
       </c>
@@ -10029,54 +9715,50 @@
       <c r="E13" s="18">
         <v>1.3698630136986301E-3</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="32">
         <f>C13*(1-Uscite!E20-Uscite!E43)</f>
-        <v>4.5660033643582648E-3</v>
+        <v>3.1963470319634705E-3</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>27</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I13" s="18">
         <v>1.0904109589041096</v>
       </c>
       <c r="J13" s="21">
         <f>1/(I$13+SUM(F13:F15))</f>
-        <v>0.20389464241010324</v>
+        <v>0.27060422587421229</v>
       </c>
       <c r="K13" s="22">
-        <f t="shared" si="0"/>
-        <v>9.3098362321915676E-4</v>
+        <f>F13*J13</f>
+        <v>8.6494501420981106E-4</v>
       </c>
       <c r="L13" s="22">
         <f>SUM(K$13:K$15)</f>
-        <v>0.77767104745418902</v>
+        <v>0.70493018658099604</v>
       </c>
       <c r="M13" s="21">
         <f>IF(MOD(ROW(),3)=1,(L13*J13)/(1-K13),IF(MOD(ROW(),3)=2,(L13*J13)/((1-K13)*(1-K13-K14)), IF(MOD(ROW(),3)=0,(L13*J13)/((1-K13-K14)*(1-L13)))))</f>
-        <v>0.15871071721191596</v>
+        <v>0.19092222466143724</v>
       </c>
       <c r="N13" s="21">
-        <f t="shared" si="1"/>
-        <v>0.36260535962201923</v>
+        <f t="shared" si="0"/>
+        <v>0.46152645053564956</v>
       </c>
       <c r="O13" s="21">
-        <f t="shared" si="2"/>
-        <v>7.2467366874932144E-4</v>
+        <f>M13*F13</f>
+        <v>6.1025368613244779E-4</v>
       </c>
       <c r="P13" s="21">
-        <f t="shared" si="3"/>
-        <v>1.6556572919684783E-3</v>
-      </c>
-      <c r="Q13" s="23">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
+        <f>N13*F13</f>
+        <v>1.4751987003422588E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="23"/>
       <c r="B14" s="17" t="s">
         <v>21</v>
       </c>
@@ -10089,52 +9771,48 @@
       <c r="E14" s="18">
         <v>0.21095890410958903</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <f>C14*(1-Uscite!E21-Uscite!E44)</f>
-        <v>2.8347404821173301</v>
+        <v>2.5634703196347033</v>
       </c>
       <c r="G14" s="19"/>
       <c r="H14" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I14" s="18">
         <v>0.87168949771689508</v>
       </c>
       <c r="J14" s="21">
         <f>J13</f>
-        <v>0.20389464241010324</v>
+        <v>0.27060422587421229</v>
       </c>
       <c r="K14" s="22">
-        <f t="shared" si="0"/>
-        <v>0.57798839692675674</v>
+        <f>F14*J14</f>
+        <v>0.6936859013962684</v>
       </c>
       <c r="L14" s="22">
         <f>L13</f>
-        <v>0.77767104745418902</v>
+        <v>0.70493018658099604</v>
       </c>
       <c r="M14" s="21">
         <f>IF(MOD(ROW(),3)=1,(L13*J13)/(1-K13),IF(MOD(ROW(),3)=2,(L13*J13)/((1-K13)*(1-K13-K14)), IF(MOD(ROW(),3)=0,(L13*J13)/((1-K13-K14)*(1-L13)))))</f>
-        <v>0.37691289952790746</v>
+        <v>0.62505403081917954</v>
       </c>
       <c r="N14" s="21">
-        <f t="shared" si="1"/>
-        <v>0.58080754193801076</v>
+        <f t="shared" si="0"/>
+        <v>0.89565825669339183</v>
       </c>
       <c r="O14" s="21">
-        <f t="shared" si="2"/>
-        <v>1.0684502545239811</v>
+        <f>M14*F14</f>
+        <v>1.602307456173002</v>
       </c>
       <c r="P14" s="21">
-        <f t="shared" si="3"/>
-        <v>1.6464386514507381</v>
-      </c>
-      <c r="Q14" s="23">
-        <f t="shared" si="4"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="24"/>
+        <f>N14*F14</f>
+        <v>2.2959933575692704</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
       <c r="B15" s="17" t="s">
         <v>23</v>
       </c>
@@ -10147,105 +9825,101 @@
       <c r="E15" s="18">
         <v>0.75570776255707761</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="32">
         <f>C15*(1-Uscite!E22-Uscite!E45)</f>
-        <v>0.97477630875878618</v>
+        <v>3.8356164383561722E-2</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I15" s="18">
         <v>0.21872146118721461</v>
       </c>
       <c r="J15" s="21">
         <f>J14</f>
-        <v>0.20389464241010324</v>
+        <v>0.27060422587421229</v>
       </c>
       <c r="K15" s="22">
-        <f t="shared" si="0"/>
-        <v>0.19875166690421309</v>
+        <f>F15*J15</f>
+        <v>1.0379340170517753E-2</v>
       </c>
       <c r="L15" s="22">
         <f>L14</f>
-        <v>0.77767104745418902</v>
+        <v>0.70493018658099604</v>
       </c>
       <c r="M15" s="21">
         <f>IF(MOD(ROW(),3)=1,(L13*J13)/(1-K13),IF(MOD(ROW(),3)=2,(L13*J13)/((1-K13)*(1-K13-K14)), IF(MOD(ROW(),3)=0,(L13*J13)/((1-K13-K14)*(1-L13)))))</f>
-        <v>1.6937155304299658</v>
+        <v>2.1164936738709748</v>
       </c>
       <c r="N15" s="21">
-        <f t="shared" si="1"/>
-        <v>1.8976101728400692</v>
+        <f t="shared" si="0"/>
+        <v>2.387097899745187</v>
       </c>
       <c r="O15" s="21">
-        <f t="shared" si="2"/>
-        <v>1.6509937728399517</v>
+        <f>M15*F15</f>
+        <v>8.1180579271763587E-2</v>
       </c>
       <c r="P15" s="21">
-        <f t="shared" si="3"/>
-        <v>1.8497454397441648</v>
-      </c>
-      <c r="Q15" s="23">
-        <f t="shared" si="4"/>
-        <v>0.29788519637462235</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
+        <f>N15*F15</f>
+        <v>9.155991944228134E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="69" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="74"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="75"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="52"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="53"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>75</v>
-      </c>
       <c r="D19" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="E19" s="30" t="s">
-        <v>59</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="30" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <f>Uscite!D55</f>
         <v>2.0547945205479451E-2</v>
       </c>
@@ -10254,67 +9928,67 @@
         <v>0.16666666666666666</v>
       </c>
       <c r="E20" s="22">
-        <f t="shared" ref="E20:E31" si="5">D20*C20</f>
+        <f t="shared" ref="E20:E31" si="4">D20*C20</f>
         <v>3.4246575342465752E-3</v>
       </c>
       <c r="F20" s="22">
-        <f t="shared" ref="F20:F31" si="6">D20</f>
+        <f t="shared" ref="F20:F31" si="5">D20</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="G20" s="22">
-        <f t="shared" ref="G20:G31" si="7">F20*C20</f>
+        <f t="shared" ref="G20:G31" si="6">F20*C20</f>
         <v>3.4246575342465752E-3</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="31">
         <f>Uscite!D56</f>
         <v>22.43013698630137</v>
       </c>
       <c r="D21" s="22">
-        <f t="shared" ref="D21:D31" si="8">4/24</f>
+        <f t="shared" ref="D21:D31" si="7">4/24</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="E21" s="22">
+        <f t="shared" si="4"/>
+        <v>3.7383561643835614</v>
+      </c>
+      <c r="F21" s="22">
         <f t="shared" si="5"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G21" s="22">
+        <f t="shared" si="6"/>
         <v>3.7383561643835614</v>
       </c>
-      <c r="F21" s="22">
-        <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G21" s="22">
-        <f t="shared" si="7"/>
-        <v>3.7383561643835614</v>
-      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="31">
         <f>Uscite!D57</f>
         <v>1.800456621004566</v>
       </c>
       <c r="D22" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E22" s="22">
+        <f t="shared" si="4"/>
+        <v>0.30007610350076097</v>
+      </c>
+      <c r="F22" s="22">
         <f t="shared" si="5"/>
-        <v>0.30007610350076097</v>
-      </c>
-      <c r="F22" s="22">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G22" s="22">
         <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G22" s="22">
-        <f t="shared" si="7"/>
         <v>0.30007610350076097</v>
       </c>
     </row>
@@ -10330,24 +10004,24 @@
         <v>1.187214611872146E-2</v>
       </c>
       <c r="D23" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E23" s="22">
+        <f t="shared" si="4"/>
+        <v>1.9786910197869098E-3</v>
+      </c>
+      <c r="F23" s="22">
         <f t="shared" si="5"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G23" s="22">
+        <f t="shared" si="6"/>
         <v>1.9786910197869098E-3</v>
       </c>
-      <c r="F23" s="22">
-        <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G23" s="22">
-        <f t="shared" si="7"/>
-        <v>1.9786910197869098E-3</v>
-      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="24"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="17" t="s">
         <v>21</v>
       </c>
@@ -10356,24 +10030,24 @@
         <v>17.739726027397261</v>
       </c>
       <c r="D24" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E24" s="22">
+        <f t="shared" si="4"/>
+        <v>2.9566210045662098</v>
+      </c>
+      <c r="F24" s="22">
         <f t="shared" si="5"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G24" s="22">
+        <f t="shared" si="6"/>
         <v>2.9566210045662098</v>
       </c>
-      <c r="F24" s="22">
-        <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G24" s="22">
-        <f t="shared" si="7"/>
-        <v>2.9566210045662098</v>
-      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="17" t="s">
         <v>23</v>
       </c>
@@ -10382,19 +10056,19 @@
         <v>1.7132420091324201</v>
       </c>
       <c r="D25" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E25" s="22">
+        <f t="shared" si="4"/>
+        <v>0.28554033485540331</v>
+      </c>
+      <c r="F25" s="22">
         <f t="shared" si="5"/>
-        <v>0.28554033485540331</v>
-      </c>
-      <c r="F25" s="22">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G25" s="22">
         <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G25" s="22">
-        <f t="shared" si="7"/>
         <v>0.28554033485540331</v>
       </c>
     </row>
@@ -10410,24 +10084,24 @@
         <v>1.0502283105022832E-2</v>
       </c>
       <c r="D26" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E26" s="22">
+        <f t="shared" si="4"/>
+        <v>1.7503805175038052E-3</v>
+      </c>
+      <c r="F26" s="22">
         <f t="shared" si="5"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G26" s="22">
+        <f t="shared" si="6"/>
         <v>1.7503805175038052E-3</v>
       </c>
-      <c r="F26" s="22">
-        <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G26" s="22">
-        <f t="shared" si="7"/>
-        <v>1.7503805175038052E-3</v>
-      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="24"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="17" t="s">
         <v>21</v>
       </c>
@@ -10436,24 +10110,24 @@
         <v>6.7986301369863016</v>
       </c>
       <c r="D27" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E27" s="22">
+        <f t="shared" si="4"/>
+        <v>1.1331050228310502</v>
+      </c>
+      <c r="F27" s="22">
         <f t="shared" si="5"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G27" s="22">
+        <f t="shared" si="6"/>
         <v>1.1331050228310502</v>
       </c>
-      <c r="F27" s="22">
-        <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G27" s="22">
-        <f t="shared" si="7"/>
-        <v>1.1331050228310502</v>
-      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="17" t="s">
         <v>23</v>
       </c>
@@ -10462,19 +10136,19 @@
         <v>0.54292237442922375</v>
       </c>
       <c r="D28" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E28" s="22">
+        <f t="shared" si="4"/>
+        <v>9.0487062404870616E-2</v>
+      </c>
+      <c r="F28" s="22">
         <f t="shared" si="5"/>
-        <v>9.0487062404870616E-2</v>
-      </c>
-      <c r="F28" s="22">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G28" s="22">
         <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G28" s="22">
-        <f t="shared" si="7"/>
         <v>9.0487062404870616E-2</v>
       </c>
     </row>
@@ -10490,24 +10164,24 @@
         <v>2.2831050228310505E-3</v>
       </c>
       <c r="D29" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E29" s="22">
+        <f t="shared" si="4"/>
+        <v>3.8051750380517507E-4</v>
+      </c>
+      <c r="F29" s="22">
         <f t="shared" si="5"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G29" s="22">
+        <f t="shared" si="6"/>
         <v>3.8051750380517507E-4</v>
       </c>
-      <c r="F29" s="22">
-        <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G29" s="22">
-        <f t="shared" si="7"/>
-        <v>3.8051750380517507E-4</v>
-      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="24"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="17" t="s">
         <v>21</v>
       </c>
@@ -10516,24 +10190,24 @@
         <v>2.4456621004566208</v>
       </c>
       <c r="D30" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E30" s="22">
+        <f t="shared" si="4"/>
+        <v>0.40761035007610347</v>
+      </c>
+      <c r="F30" s="22">
         <f t="shared" si="5"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G30" s="22">
+        <f t="shared" si="6"/>
         <v>0.40761035007610347</v>
       </c>
-      <c r="F30" s="22">
-        <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G30" s="22">
-        <f t="shared" si="7"/>
-        <v>0.40761035007610347</v>
-      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="24"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="17" t="s">
         <v>23</v>
       </c>
@@ -10542,32 +10216,32 @@
         <v>0.17899543378995433</v>
       </c>
       <c r="D31" s="22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="E31" s="22">
+        <f t="shared" si="4"/>
+        <v>2.983257229832572E-2</v>
+      </c>
+      <c r="F31" s="22">
         <f t="shared" si="5"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G31" s="22">
+        <f t="shared" si="6"/>
         <v>2.983257229832572E-2</v>
       </c>
-      <c r="F31" s="22">
-        <f t="shared" si="6"/>
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="G31" s="22">
-        <f t="shared" si="7"/>
-        <v>2.983257229832572E-2</v>
-      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="25"/>
+      <c r="D32" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A18:G18"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="K2:L2"/>
-    <mergeCell ref="A18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10576,6 +10250,905 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8A70289-E0EB-4E13-B21C-62A20F7D26A8}">
+  <dimension ref="A1:M35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="64"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="31">
+        <v>12.232876712328768</v>
+      </c>
+      <c r="C3" s="31">
+        <v>0.32265770810003735</v>
+      </c>
+      <c r="D3" s="31">
+        <v>1</v>
+      </c>
+      <c r="E3" s="34">
+        <f>B3*(1-(C3/B3)-(D3/B3))</f>
+        <v>10.910219004228731</v>
+      </c>
+      <c r="F3" s="21">
+        <f>(5*365)/2</f>
+        <v>912.5</v>
+      </c>
+      <c r="G3" s="21">
+        <f>(5*365)/2</f>
+        <v>912.5</v>
+      </c>
+      <c r="H3" s="21">
+        <f>G3*E3</f>
+        <v>9955.5748413587171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="18">
+        <v>8.6420091324200925</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0.26888935855436963</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0.88211983514741621</v>
+      </c>
+      <c r="E4" s="34">
+        <f t="shared" ref="E4:E6" si="0">B4*(1-(C4/B4)-(D4/B4))</f>
+        <v>7.4909999387183062</v>
+      </c>
+      <c r="F4" s="21">
+        <f t="shared" ref="F4:G6" si="1">(5*365)/2</f>
+        <v>912.5</v>
+      </c>
+      <c r="G4" s="21">
+        <f t="shared" si="1"/>
+        <v>912.5</v>
+      </c>
+      <c r="H4" s="21">
+        <f>G4*E4</f>
+        <v>6835.5374440804544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="18">
+        <v>3.7246575342465755</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.32548731151158516</v>
+      </c>
+      <c r="D5" s="18">
+        <v>1</v>
+      </c>
+      <c r="E5" s="34">
+        <f t="shared" si="0"/>
+        <v>2.3991702227349903</v>
+      </c>
+      <c r="F5" s="21">
+        <f t="shared" si="1"/>
+        <v>912.5</v>
+      </c>
+      <c r="G5" s="21">
+        <f t="shared" si="1"/>
+        <v>912.5</v>
+      </c>
+      <c r="H5" s="21">
+        <f>G5*E5</f>
+        <v>2189.2428282456785</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="18">
+        <v>1.0191780821917809</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.22087813620071686</v>
+      </c>
+      <c r="D6" s="18">
+        <v>0.74148745519713255</v>
+      </c>
+      <c r="E6" s="34">
+        <f t="shared" si="0"/>
+        <v>5.6812490793931421E-2</v>
+      </c>
+      <c r="F6" s="21">
+        <f t="shared" si="1"/>
+        <v>912.5</v>
+      </c>
+      <c r="G6" s="21">
+        <f t="shared" si="1"/>
+        <v>912.5</v>
+      </c>
+      <c r="H6" s="21">
+        <f>G6*E6</f>
+        <v>51.841397849462425</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="64"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="79" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="31">
+        <v>5.2054794520547946E-2</v>
+      </c>
+      <c r="D10" s="31">
+        <v>2.7397260273972603E-3</v>
+      </c>
+      <c r="E10" s="31">
+        <v>6.392694063926941E-3</v>
+      </c>
+      <c r="F10" s="78">
+        <v>4.2922374429223746E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="23"/>
+      <c r="B11" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="18">
+        <v>37.6803652968037</v>
+      </c>
+      <c r="D11" s="18">
+        <v>2.5036529680365298</v>
+      </c>
+      <c r="E11" s="18">
+        <v>4.1684931506849319</v>
+      </c>
+      <c r="F11" s="76">
+        <v>31.008219178082197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="18">
+        <v>2.9223744292237442E-2</v>
+      </c>
+      <c r="D12" s="18">
+        <v>9.1324200913242006E-4</v>
+      </c>
+      <c r="E12" s="18">
+        <v>1.3698630136986301E-3</v>
+      </c>
+      <c r="F12" s="76">
+        <v>2.6940639269406392E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="18">
+        <v>24.666210045662098</v>
+      </c>
+      <c r="D13" s="18">
+        <v>1.2205479452054795</v>
+      </c>
+      <c r="E13" s="18">
+        <v>2.3378995433789957</v>
+      </c>
+      <c r="F13" s="76">
+        <v>21.107762557077624</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="18">
+        <v>1.643835616438356E-2</v>
+      </c>
+      <c r="D14" s="18">
+        <v>0</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0</v>
+      </c>
+      <c r="F14" s="76">
+        <v>1.643835616438356E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="23"/>
+      <c r="B15" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="18">
+        <v>11.501369863013698</v>
+      </c>
+      <c r="D15" s="18">
+        <v>0.77579908675799092</v>
+      </c>
+      <c r="E15" s="18">
+        <v>1.2438356164383562</v>
+      </c>
+      <c r="F15" s="76">
+        <v>9.4817351598173527</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="18">
+        <v>4.5662100456621011E-3</v>
+      </c>
+      <c r="D16" s="18">
+        <v>0</v>
+      </c>
+      <c r="E16" s="18">
+        <v>1.3698630136986301E-3</v>
+      </c>
+      <c r="F16" s="76">
+        <v>3.1963470319634705E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+      <c r="B17" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="18">
+        <v>2.8799086757990868</v>
+      </c>
+      <c r="D17" s="18">
+        <v>0.10547945205479452</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0.21095890410958903</v>
+      </c>
+      <c r="F17" s="76">
+        <v>2.5634703196347033</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="33"/>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="63"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="70" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="71"/>
+      <c r="L19" s="71"/>
+      <c r="M19" s="72"/>
+    </row>
+    <row r="20" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="68"/>
+      <c r="J20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="31">
+        <v>22.411872146118721</v>
+      </c>
+      <c r="E21" s="50"/>
+      <c r="F21" s="51"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="49"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="18">
+        <v>12.106849315068493</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="22">
+        <f>1/(C$21)</f>
+        <v>4.4619208671203295E-2</v>
+      </c>
+      <c r="H22" s="22" t="e">
+        <f>#REF!*G22</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I22" s="22" t="e">
+        <f>SUM(H22:H23)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J22" s="22" t="e">
+        <f>IF(F22="Critical",(I22*G22)/(1-H22),IF(F22="Normal",(I22*G22)/((1-H21)*(1-I22))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K22" s="22" t="e">
+        <f>J22+G22</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L22" s="22" t="e">
+        <f>J22*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M22" s="22" t="e">
+        <f>K22*#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" s="18">
+        <v>10.305022831050229</v>
+      </c>
+      <c r="E23" s="23"/>
+      <c r="F23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="21">
+        <f>G22</f>
+        <v>4.4619208671203295E-2</v>
+      </c>
+      <c r="H23" s="22" t="e">
+        <f>#REF!*G23</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I23" s="22" t="e">
+        <f>I22</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J23" s="22" t="e">
+        <f>IF(F23="Critical",(I23*G23)/(1-H23),IF(F23="Normal",(I23*G23)/((1-H22)*(1-I23))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K23" s="22" t="e">
+        <f t="shared" ref="K23:K29" si="2">J23+G23</f>
+        <v>#REF!</v>
+      </c>
+      <c r="L23" s="22" t="e">
+        <f>J23*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M23" s="22" t="e">
+        <f>K23*#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="18">
+        <v>13.938356164383562</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="21">
+        <f>1/(C24)</f>
+        <v>7.1744471744471738E-2</v>
+      </c>
+      <c r="H24" s="22" t="e">
+        <f>#REF!*G24</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I24" s="22" t="e">
+        <f>SUM(H24:H25)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J24" s="22" t="e">
+        <f t="shared" ref="J24:J29" si="3">IF(F24="Critical",(I24*G24)/(1-H24),IF(F24="Normal",(I24*G24)/((1-H23)*(1-I24))))</f>
+        <v>#REF!</v>
+      </c>
+      <c r="K24" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L24" s="22" t="e">
+        <f>J24*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M24" s="22" t="e">
+        <f>K24*#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="18">
+        <v>9.3986301369863021</v>
+      </c>
+      <c r="E25" s="23"/>
+      <c r="F25" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="21">
+        <f>G24</f>
+        <v>7.1744471744471738E-2</v>
+      </c>
+      <c r="H25" s="22" t="e">
+        <f>#REF!*G25</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I25" s="22" t="e">
+        <f>I24</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J25" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K25" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L25" s="22" t="e">
+        <f>J25*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M25" s="22" t="e">
+        <f>K25*#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="18">
+        <v>4.5397260273972604</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="21">
+        <f>1/(C27)</f>
+        <v>0.2312565997888068</v>
+      </c>
+      <c r="H26" s="22" t="e">
+        <f>#REF!*G26</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I26" s="21" t="e">
+        <f>SUM(H26:H27)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J26" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K26" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L26" s="22" t="e">
+        <f>J26*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M26" s="22" t="e">
+        <f>K26*#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="18">
+        <v>4.3242009132420085</v>
+      </c>
+      <c r="E27" s="23"/>
+      <c r="F27" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" s="21">
+        <f>G26</f>
+        <v>0.2312565997888068</v>
+      </c>
+      <c r="H27" s="22" t="e">
+        <f>#REF!*G27</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I27" s="21" t="e">
+        <f>I26</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J27" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K27" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L27" s="22" t="e">
+        <f>J27*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M27" s="22" t="e">
+        <f>K27*#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="18">
+        <v>2.9876712328767123</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="21">
+        <f>1/(C30)</f>
+        <v>0.91708542713567842</v>
+      </c>
+      <c r="H28" s="22" t="e">
+        <f>#REF!*G28</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I28" s="21" t="e">
+        <f>SUM(H28:H29)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J28" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K28" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L28" s="22" t="e">
+        <f>J28*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M28" s="22" t="e">
+        <f>K28*#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="18">
+        <v>1.3365296803652968</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" s="21">
+        <f>G28</f>
+        <v>0.91708542713567842</v>
+      </c>
+      <c r="H29" s="22" t="e">
+        <f>#REF!*G29</f>
+        <v>#REF!</v>
+      </c>
+      <c r="I29" s="21" t="e">
+        <f>I28</f>
+        <v>#REF!</v>
+      </c>
+      <c r="J29" s="22" t="e">
+        <f t="shared" si="3"/>
+        <v>#REF!</v>
+      </c>
+      <c r="K29" s="22" t="e">
+        <f t="shared" si="2"/>
+        <v>#REF!</v>
+      </c>
+      <c r="L29" s="22" t="e">
+        <f>J29*#REF!</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M29" s="22" t="e">
+        <f>K29*#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="18">
+        <v>1.0904109589041096</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
+      <c r="K30" s="24"/>
+      <c r="L30" s="24"/>
+      <c r="M30" s="24"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="19"/>
+      <c r="B31" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="18">
+        <v>0.87168949771689508</v>
+      </c>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
+      <c r="K31" s="24"/>
+      <c r="L31" s="24"/>
+      <c r="M31" s="24"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="19"/>
+      <c r="B32" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="18">
+        <v>0.21872146118721461</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="24"/>
+      <c r="L34" s="24"/>
+      <c r="M34" s="24"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E35" s="33"/>
+      <c r="F35" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="E19:M19"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A6:C6"/>
   <sheetViews>
@@ -10590,11 +11163,11 @@
   </cols>
   <sheetData>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="54"/>
-      <c r="C6" s="54"/>
+      <c r="A6" s="73" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>